<commit_message>
updated login module and updated the frame work
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="register" sheetId="2" r:id="rId2"/>
-    <sheet name="code" sheetId="3" r:id="rId3"/>
+    <sheet name="code" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>username</t>
   </si>
@@ -55,13 +54,172 @@
   </si>
   <si>
     <t>NumpyNinja</t>
+  </si>
+  <si>
+    <t>Ilike swEEt5</t>
+  </si>
+  <si>
+    <t>rabi%di3</t>
+  </si>
+  <si>
+    <t>Panipuri</t>
+  </si>
+  <si>
+    <t>Actionsquad</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Assessment</t>
+  </si>
+  <si>
+    <t>Error Msg</t>
+  </si>
+  <si>
+    <t>Numpy Ninja</t>
+  </si>
+  <si>
+    <t>Data Structures-Introduction</t>
+  </si>
+  <si>
+    <t>Time Complexity</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Arrays in Python</t>
+  </si>
+  <si>
+    <t>Arrays Using List</t>
+  </si>
+  <si>
+    <t>Basic Operations in Lists</t>
+  </si>
+  <si>
+    <t>Applications of Array</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Creating Linked LIst</t>
+  </si>
+  <si>
+    <t>Types of Linked List</t>
+  </si>
+  <si>
+    <t>Implement Linked List in Python</t>
+  </si>
+  <si>
+    <t>Traversal</t>
+  </si>
+  <si>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>Deletion</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Operations in Stack</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Implementation of Queue in Python</t>
+  </si>
+  <si>
+    <t>Implementation using collections.deque</t>
+  </si>
+  <si>
+    <t>Implementation using array</t>
+  </si>
+  <si>
+    <t>Queue Operations</t>
+  </si>
+  <si>
+    <t>Terminologies</t>
+  </si>
+  <si>
+    <t>Types of Trees</t>
+  </si>
+  <si>
+    <t>Tree Traversals</t>
+  </si>
+  <si>
+    <t>Traversals-Illustration</t>
+  </si>
+  <si>
+    <t>Binary Trees</t>
+  </si>
+  <si>
+    <t>Types of Binary Trees</t>
+  </si>
+  <si>
+    <t>Implementation in Python</t>
+  </si>
+  <si>
+    <t>Binary Tree Traversals</t>
+  </si>
+  <si>
+    <t>Implementation of Binary Trees</t>
+  </si>
+  <si>
+    <t>Applications of Binary trees</t>
+  </si>
+  <si>
+    <t>Binary Search Trees</t>
+  </si>
+  <si>
+    <t>Implementation Of BST</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Graph Representations</t>
+  </si>
+  <si>
+    <t>Practice Questions</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>invalidcode</t>
+  </si>
+  <si>
+    <t>print("ACTION SQUAD")</t>
+  </si>
+  <si>
+    <t>print("Hello</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>ACTION SQUAD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,16 +235,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,14 +270,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -407,21 +607,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5703125" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +637,17 @@
       <c r="D1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -448,8 +660,17 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -463,9 +684,232 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -482,24 +926,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
LL and Queue Steps updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FB0F5173-F269-4C9C-8981-73D262CF8FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="code" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="E1:T27"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>username</t>
   </si>
@@ -213,12 +215,15 @@
   </si>
   <si>
     <t>ACTION SQUAD</t>
+  </si>
+  <si>
+    <t>Logged out successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,6 +401,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -431,6 +453,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -606,25 +645,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" customWidth="1"/>
+    <col min="1" max="1" width="42.5546875" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +686,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -670,7 +709,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -684,7 +723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -695,7 +734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -709,212 +748,215 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D19" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D20" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D22" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D24" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D25" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D26" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D28" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D29" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D30" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D31" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D32" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D33" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D34" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D35" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D36" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D37" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D38" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D40" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D41" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D42" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D43" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D44" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D45" s="3" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -922,14 +964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel List spelling change
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7894D5A0-C75A-4D75-ACD2-594E63BA9D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -104,9 +105,6 @@
     <t>Introduction</t>
   </si>
   <si>
-    <t>Creating Linked LIst</t>
-  </si>
-  <si>
     <t>Types of Linked List</t>
   </si>
   <si>
@@ -249,12 +247,15 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>Creating Linked List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,6 +447,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -481,6 +499,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -656,26 +691,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5546875" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,16 +724,16 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
-        <v>60</v>
-      </c>
       <c r="G1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -712,16 +747,16 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
       <c r="G2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -735,21 +770,21 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -763,248 +798,248 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
         <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>71</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="3" t="s">
+    <row r="18" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="3" t="s">
+    <row r="19" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="3" t="s">
+    <row r="20" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="3" t="s">
+    <row r="21" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="2" t="s">
+    <row r="22" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="2" t="s">
+    <row r="23" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="4" t="s">
+    <row r="24" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="4" t="s">
+    <row r="25" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="3" t="s">
+    <row r="26" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="2" t="s">
+    <row r="27" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="3" t="s">
+    <row r="28" spans="4:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="3" t="s">
+    <row r="29" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="3" t="s">
+    <row r="30" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="3" t="s">
+    <row r="31" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="3" t="s">
+    <row r="32" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D32" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="3" t="s">
+    <row r="33" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="3" t="s">
+    <row r="34" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="3" t="s">
+    <row r="35" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="2" t="s">
+    <row r="36" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="2" t="s">
+    <row r="37" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="2" t="s">
+    <row r="38" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="3" t="s">
+    <row r="39" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="3" t="s">
+    <row r="40" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D40" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="3" t="s">
+    <row r="41" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="3" t="s">
+    <row r="42" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D42" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="3" t="s">
+    <row r="43" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="2" t="s">
+    <row r="44" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D44" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="3" t="s">
+    <row r="45" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D45" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A8" r:id="rId2" display="ActionSquad@#%^&amp;"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A8" r:id="rId2" display="ActionSquad@#%^&amp;" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1012,14 +1047,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated Array, try editor and Test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7894D5A0-C75A-4D75-ACD2-594E63BA9D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="2235" windowWidth="17280" windowHeight="9960"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="code" sheetId="2" r:id="rId2"/>
+    <sheet name="code" sheetId="5" r:id="rId2"/>
+    <sheet name="python" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
   <si>
     <t>username</t>
   </si>
@@ -249,14 +249,120 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Creating Linked List</t>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://dsportalapp.herokuapp.com/question/1</t>
+  </si>
+  <si>
+    <t>https://dsportalapp.herokuapp.com/question/2</t>
+  </si>
+  <si>
+    <t>https://dsportalapp.herokuapp.com/question/3</t>
+  </si>
+  <si>
+    <t>https://dsportalapp.herokuapp.com/question/4</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+\b
+\b
+else:
+count+= 1
+\b
+\b
+result = max(result, count)
+\b
+\b
+print(result)
+\b
+\b
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+\b
+\b
+\b
+\b
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 2</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>pythoncode</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Creating Linked LIst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,8 +390,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,8 +415,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -333,12 +456,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -353,10 +492,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -447,23 +593,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -499,23 +628,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -691,26 +803,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.5546875" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +845,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -756,7 +868,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -772,8 +884,11 @@
       <c r="F3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -783,8 +898,11 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -798,7 +916,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -809,7 +927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -820,7 +938,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
@@ -831,7 +949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>71</v>
       </c>
@@ -839,7 +957,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>72</v>
       </c>
@@ -847,7 +965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>73</v>
       </c>
@@ -855,7 +973,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>74</v>
       </c>
@@ -863,7 +981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>75</v>
       </c>
@@ -871,175 +989,178 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="4:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D43" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A8" r:id="rId2" display="ActionSquad@#%^&amp;" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="A8" r:id="rId2" display="ActionSquad@#%^&amp;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1047,15 +1168,138 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="243.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>